<commit_message>
showing forecast after rec bolus is implemented
</commit_message>
<xml_diff>
--- a/example_files/dosing-threshold-example-1.xlsx
+++ b/example_files/dosing-threshold-example-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/projects/PyLoopKit/example_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7843E33E-C05B-1C4D-815B-FB075FE2D4DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418EDB1E-BAF6-A442-A1FB-651DCECDC37D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="31300" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34780" yWindow="-5560" windowWidth="31300" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -1062,10 +1062,10 @@
   <dimension ref="A1:EI46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>